<commit_message>
aprobada la matriz del flujo acumulado
</commit_message>
<xml_diff>
--- a/Datos/Old_Format/2025/01.ENERO/RPT_GESTION_ENERGIA_ENERO_04_2025.xlsx
+++ b/Datos/Old_Format/2025/01.ENERO/RPT_GESTION_ENERGIA_ENERO_04_2025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26015"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://edificiobancodeoccidente-my.sharepoint.com/personal/ccontrol_edificiobancodeoccidente_com_co/Documents/COMPARTIDA_CCONTROL/RPT_GESTION_DE_ENERGIA/2025/01.ENERO/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Familia\Documents\Personal\Escuela Pol. Feminista\Feministadística\GitHub\Energy\Datos\Old_Format\2025\01.ENERO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{5F7F510D-C21D-4485-8849-C4423D7C77EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB670A41-CA4D-493E-9B61-6E805732481E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEAF8F8D-903B-47D9-A296-C98337922CB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{15DB0DDD-8B46-476B-962B-17A4E6906705}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="19440" windowHeight="10320" tabRatio="500" xr2:uid="{15DB0DDD-8B46-476B-962B-17A4E6906705}"/>
   </bookViews>
   <sheets>
     <sheet name="REPORTE" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1455" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1451" uniqueCount="175">
   <si>
     <t>Card Number</t>
   </si>
@@ -472,18 +472,6 @@
     <t>5</t>
   </si>
   <si>
-    <t>Views</t>
-  </si>
-  <si>
-    <t>Sorts</t>
-  </si>
-  <si>
-    <t>Filter Management</t>
-  </si>
-  <si>
-    <t>Total:</t>
-  </si>
-  <si>
     <t>17192</t>
   </si>
   <si>
@@ -566,9 +554,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/mm/yyyy\ \ h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="165" formatCode="d/mm/yyyy\ \ h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -606,8 +593,8 @@
     <font>
       <sz val="10"/>
       <color indexed="8"/>
-      <name val="ARIAL"/>
-      <charset val="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -668,7 +655,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
@@ -686,9 +673,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -795,39 +779,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0E2841"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E8E8E8"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="156082"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="E97132"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="196B24"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0F9ED5"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="A02B93"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4EA72E"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="467886"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607D"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -879,7 +863,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -990,6 +974,13 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -998,13 +989,6 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1069,31 +1053,11 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1103,8 +1067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A9E536C-6A25-4DD3-833F-6032F62BE17D}">
   <dimension ref="A1:M7022"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:M147"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" topLeftCell="A120" workbookViewId="0">
+      <selection activeCell="A147" sqref="A147:XFD147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1127,7 +1091,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -1187,7 +1151,7 @@
       <c r="A3" t="s">
         <v>95</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="3">
         <v>45661.951701388891</v>
       </c>
       <c r="C3" t="s">
@@ -1224,7 +1188,7 @@
       <c r="A4" t="s">
         <v>95</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="3">
         <v>45661.951238425929</v>
       </c>
       <c r="C4" t="s">
@@ -1261,7 +1225,7 @@
       <c r="A5" t="s">
         <v>95</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="3">
         <v>45661.950115740743</v>
       </c>
       <c r="C5" t="s">
@@ -1298,7 +1262,7 @@
       <c r="A6" t="s">
         <v>95</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="3">
         <v>45661.94327546296</v>
       </c>
       <c r="C6" t="s">
@@ -1335,7 +1299,7 @@
       <c r="A7" t="s">
         <v>140</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="3">
         <v>45661.921770833331</v>
       </c>
       <c r="C7" t="s">
@@ -1372,7 +1336,7 @@
       <c r="A8" t="s">
         <v>142</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="3">
         <v>45661.917581018519</v>
       </c>
       <c r="C8" t="s">
@@ -1409,7 +1373,7 @@
       <c r="A9" t="s">
         <v>140</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="3">
         <v>45661.916805555556</v>
       </c>
       <c r="C9" t="s">
@@ -1444,9 +1408,9 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>153</v>
-      </c>
-      <c r="B10" s="6">
+        <v>149</v>
+      </c>
+      <c r="B10" s="3">
         <v>45661.914074074077</v>
       </c>
       <c r="C10" t="s">
@@ -1459,7 +1423,7 @@
         <v>48</v>
       </c>
       <c r="F10" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="G10" t="s">
         <v>45</v>
@@ -1481,9 +1445,9 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>153</v>
-      </c>
-      <c r="B11" s="6">
+        <v>149</v>
+      </c>
+      <c r="B11" s="3">
         <v>45661.913206018522</v>
       </c>
       <c r="C11" t="s">
@@ -1496,7 +1460,7 @@
         <v>48</v>
       </c>
       <c r="F11" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="G11" t="s">
         <v>14</v>
@@ -1518,9 +1482,9 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>153</v>
-      </c>
-      <c r="B12" s="6">
+        <v>149</v>
+      </c>
+      <c r="B12" s="3">
         <v>45661.911412037036</v>
       </c>
       <c r="C12" t="s">
@@ -1533,7 +1497,7 @@
         <v>48</v>
       </c>
       <c r="F12" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="G12" t="s">
         <v>41</v>
@@ -1557,7 +1521,7 @@
       <c r="A13" t="s">
         <v>95</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="3">
         <v>45661.891423611109</v>
       </c>
       <c r="C13" t="s">
@@ -1594,7 +1558,7 @@
       <c r="A14" t="s">
         <v>95</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="3">
         <v>45661.886481481481</v>
       </c>
       <c r="C14" t="s">
@@ -1631,7 +1595,7 @@
       <c r="A15" t="s">
         <v>95</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="3">
         <v>45661.885300925926</v>
       </c>
       <c r="C15" t="s">
@@ -1668,7 +1632,7 @@
       <c r="A16" t="s">
         <v>95</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="3">
         <v>45661.884675925925</v>
       </c>
       <c r="C16" t="s">
@@ -1705,7 +1669,7 @@
       <c r="A17" t="s">
         <v>95</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="3">
         <v>45661.876956018517</v>
       </c>
       <c r="C17" t="s">
@@ -1742,7 +1706,7 @@
       <c r="A18" t="s">
         <v>95</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="3">
         <v>45661.87641203704</v>
       </c>
       <c r="C18" t="s">
@@ -1779,7 +1743,7 @@
       <c r="A19" t="s">
         <v>145</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="3">
         <v>45661.866643518515</v>
       </c>
       <c r="C19" t="s">
@@ -1816,7 +1780,7 @@
       <c r="A20" t="s">
         <v>148</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="3">
         <v>45661.866273148145</v>
       </c>
       <c r="C20" t="s">
@@ -1853,7 +1817,7 @@
       <c r="A21" t="s">
         <v>95</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="3">
         <v>45661.862893518519</v>
       </c>
       <c r="C21" t="s">
@@ -1890,7 +1854,7 @@
       <c r="A22" t="s">
         <v>95</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="3">
         <v>45661.86246527778</v>
       </c>
       <c r="C22" t="s">
@@ -1927,7 +1891,7 @@
       <c r="A23" t="s">
         <v>95</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23" s="3">
         <v>45661.855520833335</v>
       </c>
       <c r="C23" t="s">
@@ -1964,7 +1928,7 @@
       <c r="A24" t="s">
         <v>95</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="3">
         <v>45661.855115740742</v>
       </c>
       <c r="C24" t="s">
@@ -2001,7 +1965,7 @@
       <c r="A25" t="s">
         <v>95</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B25" s="3">
         <v>45661.848101851851</v>
       </c>
       <c r="C25" t="s">
@@ -2038,7 +2002,7 @@
       <c r="A26" t="s">
         <v>95</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B26" s="3">
         <v>45661.847685185188</v>
       </c>
       <c r="C26" t="s">
@@ -2075,7 +2039,7 @@
       <c r="A27" t="s">
         <v>145</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B27" s="3">
         <v>45661.844421296293</v>
       </c>
       <c r="C27" t="s">
@@ -2112,7 +2076,7 @@
       <c r="A28" t="s">
         <v>95</v>
       </c>
-      <c r="B28" s="6">
+      <c r="B28" s="3">
         <v>45661.839849537035</v>
       </c>
       <c r="C28" t="s">
@@ -2149,7 +2113,7 @@
       <c r="A29" t="s">
         <v>95</v>
       </c>
-      <c r="B29" s="6">
+      <c r="B29" s="3">
         <v>45661.825150462966</v>
       </c>
       <c r="C29" t="s">
@@ -2186,7 +2150,7 @@
       <c r="A30" t="s">
         <v>95</v>
       </c>
-      <c r="B30" s="6">
+      <c r="B30" s="3">
         <v>45661.823252314818</v>
       </c>
       <c r="C30" t="s">
@@ -2223,7 +2187,7 @@
       <c r="A31" t="s">
         <v>95</v>
       </c>
-      <c r="B31" s="6">
+      <c r="B31" s="3">
         <v>45661.812361111108</v>
       </c>
       <c r="C31" t="s">
@@ -2260,7 +2224,7 @@
       <c r="A32" t="s">
         <v>95</v>
       </c>
-      <c r="B32" s="6">
+      <c r="B32" s="3">
         <v>45661.777488425927</v>
       </c>
       <c r="C32" t="s">
@@ -2297,7 +2261,7 @@
       <c r="A33" t="s">
         <v>110</v>
       </c>
-      <c r="B33" s="6">
+      <c r="B33" s="3">
         <v>45661.763379629629</v>
       </c>
       <c r="C33" t="s">
@@ -2334,7 +2298,7 @@
       <c r="A34" t="s">
         <v>95</v>
       </c>
-      <c r="B34" s="6">
+      <c r="B34" s="3">
         <v>45661.759895833333</v>
       </c>
       <c r="C34" t="s">
@@ -2371,7 +2335,7 @@
       <c r="A35" t="s">
         <v>108</v>
       </c>
-      <c r="B35" s="6">
+      <c r="B35" s="3">
         <v>45661.75886574074</v>
       </c>
       <c r="C35" t="s">
@@ -2408,7 +2372,7 @@
       <c r="A36" t="s">
         <v>94</v>
       </c>
-      <c r="B36" s="6">
+      <c r="B36" s="3">
         <v>45661.758773148147</v>
       </c>
       <c r="C36" t="s">
@@ -2445,7 +2409,7 @@
       <c r="A37" t="s">
         <v>108</v>
       </c>
-      <c r="B37" s="6">
+      <c r="B37" s="3">
         <v>45661.758553240739</v>
       </c>
       <c r="C37" t="s">
@@ -2482,7 +2446,7 @@
       <c r="A38" t="s">
         <v>108</v>
       </c>
-      <c r="B38" s="6">
+      <c r="B38" s="3">
         <v>45661.753969907404</v>
       </c>
       <c r="C38" t="s">
@@ -2519,7 +2483,7 @@
       <c r="A39" t="s">
         <v>108</v>
       </c>
-      <c r="B39" s="6">
+      <c r="B39" s="3">
         <v>45661.753657407404</v>
       </c>
       <c r="C39" t="s">
@@ -2556,7 +2520,7 @@
       <c r="A40" t="s">
         <v>110</v>
       </c>
-      <c r="B40" s="6">
+      <c r="B40" s="3">
         <v>45661.751828703702</v>
       </c>
       <c r="C40" t="s">
@@ -2591,7 +2555,7 @@
       <c r="A41" t="s">
         <v>94</v>
       </c>
-      <c r="B41" s="6">
+      <c r="B41" s="3">
         <v>45661.74931712963</v>
       </c>
       <c r="C41" t="s">
@@ -2628,7 +2592,7 @@
       <c r="A42" t="s">
         <v>95</v>
       </c>
-      <c r="B42" s="6">
+      <c r="B42" s="3">
         <v>45661.743414351855</v>
       </c>
       <c r="C42" t="s">
@@ -2665,7 +2629,7 @@
       <c r="A43" t="s">
         <v>95</v>
       </c>
-      <c r="B43" s="6">
+      <c r="B43" s="3">
         <v>45661.739988425928</v>
       </c>
       <c r="C43" t="s">
@@ -2702,7 +2666,7 @@
       <c r="A44" t="s">
         <v>94</v>
       </c>
-      <c r="B44" s="6">
+      <c r="B44" s="3">
         <v>45661.738576388889</v>
       </c>
       <c r="C44" t="s">
@@ -2739,7 +2703,7 @@
       <c r="A45" t="s">
         <v>112</v>
       </c>
-      <c r="B45" s="6">
+      <c r="B45" s="3">
         <v>45661.726967592593</v>
       </c>
       <c r="C45" t="s">
@@ -2776,7 +2740,7 @@
       <c r="A46" t="s">
         <v>95</v>
       </c>
-      <c r="B46" s="6">
+      <c r="B46" s="3">
         <v>45661.723009259258</v>
       </c>
       <c r="C46" t="s">
@@ -2813,7 +2777,7 @@
       <c r="A47" t="s">
         <v>112</v>
       </c>
-      <c r="B47" s="6">
+      <c r="B47" s="3">
         <v>45661.716111111113</v>
       </c>
       <c r="C47" t="s">
@@ -2850,7 +2814,7 @@
       <c r="A48" t="s">
         <v>112</v>
       </c>
-      <c r="B48" s="6">
+      <c r="B48" s="3">
         <v>45661.714571759258</v>
       </c>
       <c r="C48" t="s">
@@ -2887,7 +2851,7 @@
       <c r="A49" t="s">
         <v>108</v>
       </c>
-      <c r="B49" s="6">
+      <c r="B49" s="3">
         <v>45661.71429398148</v>
       </c>
       <c r="C49" t="s">
@@ -2924,7 +2888,7 @@
       <c r="A50" t="s">
         <v>95</v>
       </c>
-      <c r="B50" s="6">
+      <c r="B50" s="3">
         <v>45661.712951388887</v>
       </c>
       <c r="C50" t="s">
@@ -2961,7 +2925,7 @@
       <c r="A51" t="s">
         <v>130</v>
       </c>
-      <c r="B51" s="6">
+      <c r="B51" s="3">
         <v>45661.71292824074</v>
       </c>
       <c r="C51" t="s">
@@ -2998,7 +2962,7 @@
       <c r="A52" t="s">
         <v>94</v>
       </c>
-      <c r="B52" s="6">
+      <c r="B52" s="3">
         <v>45661.712395833332</v>
       </c>
       <c r="C52" t="s">
@@ -3035,7 +2999,7 @@
       <c r="A53" t="s">
         <v>108</v>
       </c>
-      <c r="B53" s="6">
+      <c r="B53" s="3">
         <v>45661.710474537038</v>
       </c>
       <c r="C53" t="s">
@@ -3072,7 +3036,7 @@
       <c r="A54" t="s">
         <v>108</v>
       </c>
-      <c r="B54" s="6">
+      <c r="B54" s="3">
         <v>45661.71020833333</v>
       </c>
       <c r="C54" t="s">
@@ -3109,7 +3073,7 @@
       <c r="A55" t="s">
         <v>95</v>
       </c>
-      <c r="B55" s="6">
+      <c r="B55" s="3">
         <v>45661.710069444445</v>
       </c>
       <c r="C55" t="s">
@@ -3146,7 +3110,7 @@
       <c r="A56" t="s">
         <v>95</v>
       </c>
-      <c r="B56" s="6">
+      <c r="B56" s="3">
         <v>45661.709409722222</v>
       </c>
       <c r="C56" t="s">
@@ -3183,7 +3147,7 @@
       <c r="A57" t="s">
         <v>112</v>
       </c>
-      <c r="B57" s="6">
+      <c r="B57" s="3">
         <v>45661.708587962959</v>
       </c>
       <c r="C57" t="s">
@@ -3220,7 +3184,7 @@
       <c r="A58" t="s">
         <v>112</v>
       </c>
-      <c r="B58" s="6">
+      <c r="B58" s="3">
         <v>45661.708252314813</v>
       </c>
       <c r="C58" t="s">
@@ -3257,7 +3221,7 @@
       <c r="A59" t="s">
         <v>94</v>
       </c>
-      <c r="B59" s="6">
+      <c r="B59" s="3">
         <v>45661.705960648149</v>
       </c>
       <c r="C59" t="s">
@@ -3294,7 +3258,7 @@
       <c r="A60" t="s">
         <v>110</v>
       </c>
-      <c r="B60" s="6">
+      <c r="B60" s="3">
         <v>45661.700092592589</v>
       </c>
       <c r="C60" t="s">
@@ -3329,7 +3293,7 @@
       <c r="A61" t="s">
         <v>136</v>
       </c>
-      <c r="B61" s="6">
+      <c r="B61" s="3">
         <v>45661.699293981481</v>
       </c>
       <c r="C61" t="s">
@@ -3366,14 +3330,14 @@
       <c r="A62" t="s">
         <v>118</v>
       </c>
-      <c r="B62" s="6">
+      <c r="B62" s="3">
         <v>45661.699259259258</v>
       </c>
       <c r="C62" t="s">
         <v>13</v>
       </c>
       <c r="D62" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="E62" t="s">
         <v>33</v>
@@ -3395,7 +3359,7 @@
         <v>77</v>
       </c>
       <c r="L62" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="M62"/>
     </row>
@@ -3403,17 +3367,17 @@
       <c r="A63" t="s">
         <v>137</v>
       </c>
-      <c r="B63" s="6">
+      <c r="B63" s="3">
         <v>45661.699236111112</v>
       </c>
       <c r="C63" t="s">
         <v>13</v>
       </c>
       <c r="D63" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E63" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F63"/>
       <c r="G63" t="s">
@@ -3432,7 +3396,7 @@
         <v>77</v>
       </c>
       <c r="L63" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="M63"/>
     </row>
@@ -3440,7 +3404,7 @@
       <c r="A64" t="s">
         <v>136</v>
       </c>
-      <c r="B64" s="6">
+      <c r="B64" s="3">
         <v>45661.698657407411</v>
       </c>
       <c r="C64" t="s">
@@ -3477,7 +3441,7 @@
       <c r="A65" t="s">
         <v>110</v>
       </c>
-      <c r="B65" s="6">
+      <c r="B65" s="3">
         <v>45661.69699074074</v>
       </c>
       <c r="C65" t="s">
@@ -3512,14 +3476,14 @@
       <c r="A66" t="s">
         <v>118</v>
       </c>
-      <c r="B66" s="6">
+      <c r="B66" s="3">
         <v>45661.687083333331</v>
       </c>
       <c r="C66" t="s">
         <v>13</v>
       </c>
       <c r="D66" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="E66" t="s">
         <v>33</v>
@@ -3541,7 +3505,7 @@
         <v>77</v>
       </c>
       <c r="L66" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="M66"/>
     </row>
@@ -3549,7 +3513,7 @@
       <c r="A67" t="s">
         <v>98</v>
       </c>
-      <c r="B67" s="6">
+      <c r="B67" s="3">
         <v>45661.683553240742</v>
       </c>
       <c r="C67" t="s">
@@ -3586,7 +3550,7 @@
       <c r="A68" t="s">
         <v>98</v>
       </c>
-      <c r="B68" s="6">
+      <c r="B68" s="3">
         <v>45661.668530092589</v>
       </c>
       <c r="C68" t="s">
@@ -3623,7 +3587,7 @@
       <c r="A69" t="s">
         <v>112</v>
       </c>
-      <c r="B69" s="6">
+      <c r="B69" s="3">
         <v>45661.668229166666</v>
       </c>
       <c r="C69" t="s">
@@ -3660,7 +3624,7 @@
       <c r="A70" t="s">
         <v>98</v>
       </c>
-      <c r="B70" s="6">
+      <c r="B70" s="3">
         <v>45661.667905092596</v>
       </c>
       <c r="C70" t="s">
@@ -3697,7 +3661,7 @@
       <c r="A71" t="s">
         <v>98</v>
       </c>
-      <c r="B71" s="6">
+      <c r="B71" s="3">
         <v>45661.667384259257</v>
       </c>
       <c r="C71" t="s">
@@ -3734,7 +3698,7 @@
       <c r="A72" t="s">
         <v>98</v>
       </c>
-      <c r="B72" s="6">
+      <c r="B72" s="3">
         <v>45661.666365740741</v>
       </c>
       <c r="C72" t="s">
@@ -3771,7 +3735,7 @@
       <c r="A73" t="s">
         <v>112</v>
       </c>
-      <c r="B73" s="6">
+      <c r="B73" s="3">
         <v>45661.666203703702</v>
       </c>
       <c r="C73" t="s">
@@ -3808,7 +3772,7 @@
       <c r="A74" t="s">
         <v>112</v>
       </c>
-      <c r="B74" s="6">
+      <c r="B74" s="3">
         <v>45661.665844907409</v>
       </c>
       <c r="C74" t="s">
@@ -3845,7 +3809,7 @@
       <c r="A75" t="s">
         <v>98</v>
       </c>
-      <c r="B75" s="6">
+      <c r="B75" s="3">
         <v>45661.658402777779</v>
       </c>
       <c r="C75" t="s">
@@ -3882,17 +3846,17 @@
       <c r="A76" t="s">
         <v>133</v>
       </c>
-      <c r="B76" s="6">
+      <c r="B76" s="3">
         <v>45661.656192129631</v>
       </c>
       <c r="C76" t="s">
         <v>13</v>
       </c>
       <c r="D76" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E76" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="F76"/>
       <c r="G76" t="s">
@@ -3908,10 +3872,10 @@
         <v>27</v>
       </c>
       <c r="K76" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="L76" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="M76"/>
     </row>
@@ -3919,7 +3883,7 @@
       <c r="A77" t="s">
         <v>138</v>
       </c>
-      <c r="B77" s="6">
+      <c r="B77" s="3">
         <v>45661.656157407408</v>
       </c>
       <c r="C77" t="s">
@@ -3956,14 +3920,14 @@
       <c r="A78" t="s">
         <v>106</v>
       </c>
-      <c r="B78" s="6">
+      <c r="B78" s="3">
         <v>45661.656111111108</v>
       </c>
       <c r="C78" t="s">
         <v>13</v>
       </c>
       <c r="D78" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E78" t="s">
         <v>75</v>
@@ -3982,10 +3946,10 @@
         <v>27</v>
       </c>
       <c r="K78" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="L78" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="M78"/>
     </row>
@@ -3993,7 +3957,7 @@
       <c r="A79" t="s">
         <v>115</v>
       </c>
-      <c r="B79" s="6">
+      <c r="B79" s="3">
         <v>45661.656076388892</v>
       </c>
       <c r="C79" t="s">
@@ -4030,17 +3994,17 @@
       <c r="A80" t="s">
         <v>132</v>
       </c>
-      <c r="B80" s="6">
+      <c r="B80" s="3">
         <v>45661.656030092592</v>
       </c>
       <c r="C80" t="s">
         <v>13</v>
       </c>
       <c r="D80" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E80" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="F80"/>
       <c r="G80" t="s">
@@ -4056,10 +4020,10 @@
         <v>27</v>
       </c>
       <c r="K80" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="L80" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="M80"/>
     </row>
@@ -4067,17 +4031,17 @@
       <c r="A81" t="s">
         <v>114</v>
       </c>
-      <c r="B81" s="6">
+      <c r="B81" s="3">
         <v>45661.655995370369</v>
       </c>
       <c r="C81" t="s">
         <v>13</v>
       </c>
       <c r="D81" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E81" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="F81"/>
       <c r="G81" t="s">
@@ -4096,7 +4060,7 @@
         <v>66</v>
       </c>
       <c r="L81" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="M81"/>
     </row>
@@ -4104,7 +4068,7 @@
       <c r="A82" t="s">
         <v>94</v>
       </c>
-      <c r="B82" s="6">
+      <c r="B82" s="3">
         <v>45661.655868055554</v>
       </c>
       <c r="C82" t="s">
@@ -4141,7 +4105,7 @@
       <c r="A83" t="s">
         <v>94</v>
       </c>
-      <c r="B83" s="6">
+      <c r="B83" s="3">
         <v>45661.655601851853</v>
       </c>
       <c r="C83" t="s">
@@ -4178,7 +4142,7 @@
       <c r="A84" t="s">
         <v>94</v>
       </c>
-      <c r="B84" s="6">
+      <c r="B84" s="3">
         <v>45661.655162037037</v>
       </c>
       <c r="C84" t="s">
@@ -4215,7 +4179,7 @@
       <c r="A85" t="s">
         <v>112</v>
       </c>
-      <c r="B85" s="6">
+      <c r="B85" s="3">
         <v>45661.654074074075</v>
       </c>
       <c r="C85" t="s">
@@ -4252,7 +4216,7 @@
       <c r="A86" t="s">
         <v>112</v>
       </c>
-      <c r="B86" s="6">
+      <c r="B86" s="3">
         <v>45661.65289351852</v>
       </c>
       <c r="C86" t="s">
@@ -4289,7 +4253,7 @@
       <c r="A87" t="s">
         <v>112</v>
       </c>
-      <c r="B87" s="6">
+      <c r="B87" s="3">
         <v>45661.652199074073</v>
       </c>
       <c r="C87" t="s">
@@ -4326,7 +4290,7 @@
       <c r="A88" t="s">
         <v>116</v>
       </c>
-      <c r="B88" s="6">
+      <c r="B88" s="3">
         <v>45661.651226851849</v>
       </c>
       <c r="C88" t="s">
@@ -4363,7 +4327,7 @@
       <c r="A89" t="s">
         <v>116</v>
       </c>
-      <c r="B89" s="6">
+      <c r="B89" s="3">
         <v>45661.648993055554</v>
       </c>
       <c r="C89" t="s">
@@ -4400,7 +4364,7 @@
       <c r="A90" t="s">
         <v>116</v>
       </c>
-      <c r="B90" s="6">
+      <c r="B90" s="3">
         <v>45661.648506944446</v>
       </c>
       <c r="C90" t="s">
@@ -4437,7 +4401,7 @@
       <c r="A91" t="s">
         <v>112</v>
       </c>
-      <c r="B91" s="6">
+      <c r="B91" s="3">
         <v>45661.647881944446</v>
       </c>
       <c r="C91" t="s">
@@ -4474,7 +4438,7 @@
       <c r="A92" t="s">
         <v>116</v>
       </c>
-      <c r="B92" s="6">
+      <c r="B92" s="3">
         <v>45661.647881944446</v>
       </c>
       <c r="C92" t="s">
@@ -4511,7 +4475,7 @@
       <c r="A93" t="s">
         <v>116</v>
       </c>
-      <c r="B93" s="6">
+      <c r="B93" s="3">
         <v>45661.647430555553</v>
       </c>
       <c r="C93" t="s">
@@ -4548,7 +4512,7 @@
       <c r="A94" t="s">
         <v>112</v>
       </c>
-      <c r="B94" s="6">
+      <c r="B94" s="3">
         <v>45661.641261574077</v>
       </c>
       <c r="C94" t="s">
@@ -4585,7 +4549,7 @@
       <c r="A95" t="s">
         <v>95</v>
       </c>
-      <c r="B95" s="6">
+      <c r="B95" s="3">
         <v>45661.638692129629</v>
       </c>
       <c r="C95" t="s">
@@ -4622,7 +4586,7 @@
       <c r="A96" t="s">
         <v>95</v>
       </c>
-      <c r="B96" s="6">
+      <c r="B96" s="3">
         <v>45661.638078703705</v>
       </c>
       <c r="C96" t="s">
@@ -4659,7 +4623,7 @@
       <c r="A97" t="s">
         <v>94</v>
       </c>
-      <c r="B97" s="6">
+      <c r="B97" s="3">
         <v>45661.636053240742</v>
       </c>
       <c r="C97" t="s">
@@ -4696,7 +4660,7 @@
       <c r="A98" t="s">
         <v>94</v>
       </c>
-      <c r="B98" s="6">
+      <c r="B98" s="3">
         <v>45661.630023148151</v>
       </c>
       <c r="C98" t="s">
@@ -4733,7 +4697,7 @@
       <c r="A99" t="s">
         <v>112</v>
       </c>
-      <c r="B99" s="6">
+      <c r="B99" s="3">
         <v>45661.627592592595</v>
       </c>
       <c r="C99" t="s">
@@ -4770,7 +4734,7 @@
       <c r="A100" t="s">
         <v>112</v>
       </c>
-      <c r="B100" s="6">
+      <c r="B100" s="3">
         <v>45661.627268518518</v>
       </c>
       <c r="C100" t="s">
@@ -4807,7 +4771,7 @@
       <c r="A101" t="s">
         <v>135</v>
       </c>
-      <c r="B101" s="6">
+      <c r="B101" s="3">
         <v>45661.625115740739</v>
       </c>
       <c r="C101" t="s">
@@ -4844,14 +4808,14 @@
       <c r="A102" t="s">
         <v>131</v>
       </c>
-      <c r="B102" s="6">
+      <c r="B102" s="3">
         <v>45661.625069444446</v>
       </c>
       <c r="C102" t="s">
         <v>13</v>
       </c>
       <c r="D102" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E102" t="s">
         <v>128</v>
@@ -4873,7 +4837,7 @@
         <v>97</v>
       </c>
       <c r="L102" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="M102"/>
     </row>
@@ -4881,14 +4845,14 @@
       <c r="A103" t="s">
         <v>123</v>
       </c>
-      <c r="B103" s="6">
+      <c r="B103" s="3">
         <v>45661.624780092592</v>
       </c>
       <c r="C103" t="s">
         <v>13</v>
       </c>
       <c r="D103" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E103" t="s">
         <v>100</v>
@@ -4907,10 +4871,10 @@
         <v>27</v>
       </c>
       <c r="K103" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="L103" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="M103"/>
     </row>
@@ -4918,7 +4882,7 @@
       <c r="A104" t="s">
         <v>95</v>
       </c>
-      <c r="B104" s="6">
+      <c r="B104" s="3">
         <v>45661.6172337963</v>
       </c>
       <c r="C104" t="s">
@@ -4955,7 +4919,7 @@
       <c r="A105" t="s">
         <v>95</v>
       </c>
-      <c r="B105" s="6">
+      <c r="B105" s="3">
         <v>45661.616863425923</v>
       </c>
       <c r="C105" t="s">
@@ -4992,7 +4956,7 @@
       <c r="A106" t="s">
         <v>95</v>
       </c>
-      <c r="B106" s="6">
+      <c r="B106" s="3">
         <v>45661.615115740744</v>
       </c>
       <c r="C106" t="s">
@@ -5029,7 +4993,7 @@
       <c r="A107" t="s">
         <v>95</v>
       </c>
-      <c r="B107" s="6">
+      <c r="B107" s="3">
         <v>45661.614791666667</v>
       </c>
       <c r="C107" t="s">
@@ -5066,17 +5030,17 @@
       <c r="A108" t="s">
         <v>137</v>
       </c>
-      <c r="B108" s="6">
+      <c r="B108" s="3">
         <v>45661.610694444447</v>
       </c>
       <c r="C108" t="s">
         <v>13</v>
       </c>
       <c r="D108" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E108" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F108"/>
       <c r="G108" t="s">
@@ -5095,7 +5059,7 @@
         <v>77</v>
       </c>
       <c r="L108" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="M108"/>
     </row>
@@ -5103,7 +5067,7 @@
       <c r="A109" t="s">
         <v>143</v>
       </c>
-      <c r="B109" s="6">
+      <c r="B109" s="3">
         <v>45661.606863425928</v>
       </c>
       <c r="C109" t="s">
@@ -5140,7 +5104,7 @@
       <c r="A110" t="s">
         <v>112</v>
       </c>
-      <c r="B110" s="6">
+      <c r="B110" s="3">
         <v>45661.601122685184</v>
       </c>
       <c r="C110" t="s">
@@ -5177,7 +5141,7 @@
       <c r="A111" t="s">
         <v>112</v>
       </c>
-      <c r="B111" s="6">
+      <c r="B111" s="3">
         <v>45661.600300925929</v>
       </c>
       <c r="C111" t="s">
@@ -5212,9 +5176,9 @@
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>155</v>
-      </c>
-      <c r="B112" s="6">
+        <v>151</v>
+      </c>
+      <c r="B112" s="3">
         <v>45661.599386574075</v>
       </c>
       <c r="C112" t="s">
@@ -5251,7 +5215,7 @@
       <c r="A113" t="s">
         <v>102</v>
       </c>
-      <c r="B113" s="6">
+      <c r="B113" s="3">
         <v>45661.599386574075</v>
       </c>
       <c r="C113" t="s">
@@ -5286,9 +5250,9 @@
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>155</v>
-      </c>
-      <c r="B114" s="6">
+        <v>151</v>
+      </c>
+      <c r="B114" s="3">
         <v>45661.59878472222</v>
       </c>
       <c r="C114" t="s">
@@ -5325,7 +5289,7 @@
       <c r="A115" t="s">
         <v>112</v>
       </c>
-      <c r="B115" s="6">
+      <c r="B115" s="3">
         <v>45661.596192129633</v>
       </c>
       <c r="C115" t="s">
@@ -5362,7 +5326,7 @@
       <c r="A116" t="s">
         <v>112</v>
       </c>
-      <c r="B116" s="6">
+      <c r="B116" s="3">
         <v>45661.59574074074</v>
       </c>
       <c r="C116" t="s">
@@ -5399,7 +5363,7 @@
       <c r="A117" t="s">
         <v>112</v>
       </c>
-      <c r="B117" s="6">
+      <c r="B117" s="3">
         <v>45661.594502314816</v>
       </c>
       <c r="C117" t="s">
@@ -5436,7 +5400,7 @@
       <c r="A118" t="s">
         <v>116</v>
       </c>
-      <c r="B118" s="6">
+      <c r="B118" s="3">
         <v>45661.587094907409</v>
       </c>
       <c r="C118" t="s">
@@ -5473,7 +5437,7 @@
       <c r="A119" t="s">
         <v>116</v>
       </c>
-      <c r="B119" s="6">
+      <c r="B119" s="3">
         <v>45661.586875000001</v>
       </c>
       <c r="C119" t="s">
@@ -5510,7 +5474,7 @@
       <c r="A120" t="s">
         <v>102</v>
       </c>
-      <c r="B120" s="6">
+      <c r="B120" s="3">
         <v>45661.582129629627</v>
       </c>
       <c r="C120" t="s">
@@ -5547,7 +5511,7 @@
       <c r="A121" t="s">
         <v>102</v>
       </c>
-      <c r="B121" s="6">
+      <c r="B121" s="3">
         <v>45661.581620370373</v>
       </c>
       <c r="C121" t="s">
@@ -5584,7 +5548,7 @@
       <c r="A122" t="s">
         <v>112</v>
       </c>
-      <c r="B122" s="6">
+      <c r="B122" s="3">
         <v>45661.573888888888</v>
       </c>
       <c r="C122" t="s">
@@ -5621,7 +5585,7 @@
       <c r="A123" t="s">
         <v>101</v>
       </c>
-      <c r="B123" s="6">
+      <c r="B123" s="3">
         <v>45661.573483796295</v>
       </c>
       <c r="C123" t="s">
@@ -5658,7 +5622,7 @@
       <c r="A124" t="s">
         <v>112</v>
       </c>
-      <c r="B124" s="6">
+      <c r="B124" s="3">
         <v>45661.57340277778</v>
       </c>
       <c r="C124" t="s">
@@ -5695,7 +5659,7 @@
       <c r="A125" t="s">
         <v>142</v>
       </c>
-      <c r="B125" s="6">
+      <c r="B125" s="3">
         <v>45661.572141203702</v>
       </c>
       <c r="C125" t="s">
@@ -5732,7 +5696,7 @@
       <c r="A126" t="s">
         <v>140</v>
       </c>
-      <c r="B126" s="6">
+      <c r="B126" s="3">
         <v>45661.571400462963</v>
       </c>
       <c r="C126" t="s">
@@ -5769,7 +5733,7 @@
       <c r="A127" t="s">
         <v>140</v>
       </c>
-      <c r="B127" s="6">
+      <c r="B127" s="3">
         <v>45661.5700462963</v>
       </c>
       <c r="C127" t="s">
@@ -5806,7 +5770,7 @@
       <c r="A128" t="s">
         <v>102</v>
       </c>
-      <c r="B128" s="6">
+      <c r="B128" s="3">
         <v>45661.569560185184</v>
       </c>
       <c r="C128" t="s">
@@ -5843,7 +5807,7 @@
       <c r="A129" t="s">
         <v>112</v>
       </c>
-      <c r="B129" s="6">
+      <c r="B129" s="3">
         <v>45661.569224537037</v>
       </c>
       <c r="C129" t="s">
@@ -5880,7 +5844,7 @@
       <c r="A130" t="s">
         <v>102</v>
       </c>
-      <c r="B130" s="6">
+      <c r="B130" s="3">
         <v>45661.569155092591</v>
       </c>
       <c r="C130" t="s">
@@ -5917,7 +5881,7 @@
       <c r="A131" t="s">
         <v>112</v>
       </c>
-      <c r="B131" s="6">
+      <c r="B131" s="3">
         <v>45661.568506944444</v>
       </c>
       <c r="C131" t="s">
@@ -5954,7 +5918,7 @@
       <c r="A132" t="s">
         <v>108</v>
       </c>
-      <c r="B132" s="6">
+      <c r="B132" s="3">
         <v>45661.567916666667</v>
       </c>
       <c r="C132" t="s">
@@ -5991,7 +5955,7 @@
       <c r="A133" t="s">
         <v>112</v>
       </c>
-      <c r="B133" s="6">
+      <c r="B133" s="3">
         <v>45661.567777777775</v>
       </c>
       <c r="C133" t="s">
@@ -6028,7 +5992,7 @@
       <c r="A134" t="s">
         <v>112</v>
       </c>
-      <c r="B134" s="6">
+      <c r="B134" s="3">
         <v>45661.567395833335</v>
       </c>
       <c r="C134" t="s">
@@ -6065,7 +6029,7 @@
       <c r="A135" t="s">
         <v>108</v>
       </c>
-      <c r="B135" s="6">
+      <c r="B135" s="3">
         <v>45661.567314814813</v>
       </c>
       <c r="C135" t="s">
@@ -6081,7 +6045,7 @@
         <v>109</v>
       </c>
       <c r="G135" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="H135" t="s">
         <v>83</v>
@@ -6102,7 +6066,7 @@
       <c r="A136" t="s">
         <v>108</v>
       </c>
-      <c r="B136" s="6">
+      <c r="B136" s="3">
         <v>45661.566458333335</v>
       </c>
       <c r="C136" t="s">
@@ -6139,7 +6103,7 @@
       <c r="A137" t="s">
         <v>102</v>
       </c>
-      <c r="B137" s="6">
+      <c r="B137" s="3">
         <v>45661.564050925925</v>
       </c>
       <c r="C137" t="s">
@@ -6176,7 +6140,7 @@
       <c r="A138" t="s">
         <v>102</v>
       </c>
-      <c r="B138" s="6">
+      <c r="B138" s="3">
         <v>45661.563587962963</v>
       </c>
       <c r="C138" t="s">
@@ -6213,7 +6177,7 @@
       <c r="A139" t="s">
         <v>102</v>
       </c>
-      <c r="B139" s="6">
+      <c r="B139" s="3">
         <v>45661.558715277781</v>
       </c>
       <c r="C139" t="s">
@@ -6250,7 +6214,7 @@
       <c r="A140" t="s">
         <v>102</v>
       </c>
-      <c r="B140" s="6">
+      <c r="B140" s="3">
         <v>45661.558252314811</v>
       </c>
       <c r="C140" t="s">
@@ -6287,7 +6251,7 @@
       <c r="A141" t="s">
         <v>102</v>
       </c>
-      <c r="B141" s="6">
+      <c r="B141" s="3">
         <v>45661.548518518517</v>
       </c>
       <c r="C141" t="s">
@@ -6324,7 +6288,7 @@
       <c r="A142" t="s">
         <v>102</v>
       </c>
-      <c r="B142" s="6">
+      <c r="B142" s="3">
         <v>45661.547939814816</v>
       </c>
       <c r="C142" t="s">
@@ -6361,7 +6325,7 @@
       <c r="A143" t="s">
         <v>101</v>
       </c>
-      <c r="B143" s="6">
+      <c r="B143" s="3">
         <v>45661.546944444446</v>
       </c>
       <c r="C143" t="s">
@@ -6398,7 +6362,7 @@
       <c r="A144" t="s">
         <v>101</v>
       </c>
-      <c r="B144" s="6">
+      <c r="B144" s="3">
         <v>45661.546018518522</v>
       </c>
       <c r="C144" t="s">
@@ -6435,7 +6399,7 @@
       <c r="A145" t="s">
         <v>115</v>
       </c>
-      <c r="B145" s="6">
+      <c r="B145" s="3">
         <v>45661.542708333334</v>
       </c>
       <c r="C145" t="s">
@@ -6472,14 +6436,14 @@
       <c r="A146" t="s">
         <v>106</v>
       </c>
-      <c r="B146" s="6">
+      <c r="B146" s="3">
         <v>45661.542002314818</v>
       </c>
       <c r="C146" t="s">
         <v>13</v>
       </c>
       <c r="D146" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E146" t="s">
         <v>75</v>
@@ -6498,30 +6462,20 @@
         <v>27</v>
       </c>
       <c r="K146" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="L146" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="M146"/>
     </row>
     <row r="147" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A147" t="s">
-        <v>149</v>
-      </c>
-      <c r="B147" t="s">
-        <v>150</v>
-      </c>
-      <c r="C147" t="s">
-        <v>151</v>
-      </c>
+      <c r="A147"/>
+      <c r="B147"/>
+      <c r="C147"/>
       <c r="D147"/>
-      <c r="E147" t="s">
-        <v>152</v>
-      </c>
-      <c r="F147" s="4">
-        <v>144</v>
-      </c>
+      <c r="E147"/>
+      <c r="F147" s="4"/>
       <c r="G147"/>
       <c r="H147"/>
       <c r="I147"/>

</xml_diff>